<commit_message>
Creacion procesos GPO.006.002 y GPO.006.003
</commit_message>
<xml_diff>
--- a/Data/Hoja de recursos.xlsx
+++ b/Data/Hoja de recursos.xlsx
@@ -1,19 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2E4Q4LA\Documents\UiPath\GeneracionCorreos_Beeckerco\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{239725AE-F449-4E5A-AE66-E98F573AD9EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Insumos" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="EjemploProcesados" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="EjemploNoProcesados" sheetId="3" r:id="rId6"/>
+    <sheet name="Insumos" sheetId="1" r:id="rId1"/>
+    <sheet name="EjemploProcesados" sheetId="2" r:id="rId2"/>
+    <sheet name="EjemploNoProcesados" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
   <si>
     <t>Nombre</t>
   </si>
@@ -51,12 +60,6 @@
     <t>Correo Electrónico</t>
   </si>
   <si>
-    <t>ivan.garcia@beeckerco.com</t>
-  </si>
-  <si>
-    <t>ivan.hernandez@beeckerco.com</t>
-  </si>
-  <si>
     <t>Descripción</t>
   </si>
   <si>
@@ -67,26 +70,37 @@
   </si>
   <si>
     <t>Sin apellido Paterno</t>
+  </si>
+  <si>
+    <t>IvánGarcía@beeckerco.com</t>
+  </si>
+  <si>
+    <t>AllissonFlores@beeckerco.com</t>
+  </si>
+  <si>
+    <t>Eunice@beeckerco.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -97,11 +111,17 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -115,47 +135,37 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -345,26 +355,171 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D8" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="38.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="13.38"/>
-    <col customWidth="1" min="2" max="2" width="15.5"/>
-    <col customWidth="1" min="3" max="3" width="15.25"/>
-    <col customWidth="1" min="4" max="4" width="25.75"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -374,134 +529,13 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="D8" s="2"/>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="1" max="1" width="38.13"/>
-    <col customWidth="1" min="2" max="2" width="18.63"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2">
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="s">
         <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="2" max="2" width="14.0"/>
-    <col customWidth="1" min="3" max="3" width="15.0"/>
-    <col customWidth="1" min="4" max="4" width="28.5"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>8</v>
@@ -510,10 +544,10 @@
         <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -522,10 +556,10 @@
         <v>6</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Falta solo la parte donde envie el correo
</commit_message>
<xml_diff>
--- a/Data/Hoja de recursos.xlsx
+++ b/Data/Hoja de recursos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Desktop\importante\Generacion-Correo-Equipo-4\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01987C3-A9BB-4081-922C-DA0A504D174B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{247F5EB0-B917-4DAC-B7CE-1D089AD01D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Insumos" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t>Nombre</t>
   </si>
@@ -61,15 +61,6 @@
   </si>
   <si>
     <t>Descripción</t>
-  </si>
-  <si>
-    <t>luis</t>
-  </si>
-  <si>
-    <t>estela</t>
-  </si>
-  <si>
-    <t>jimenez</t>
   </si>
 </sst>
 </file>
@@ -369,8 +360,8 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -446,15 +437,9 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -469,7 +454,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F13" sqref="F13:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -478,15 +463,15 @@
     <col min="2" max="2" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
     </row>
   </sheetData>
@@ -501,7 +486,7 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="A2:D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Ya no mover validaciones o lo hechan a perder
</commit_message>
<xml_diff>
--- a/Data/Hoja de recursos.xlsx
+++ b/Data/Hoja de recursos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Desktop\importante\Generacion-Correo-Equipo-4\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{247F5EB0-B917-4DAC-B7CE-1D089AD01D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF99F3A-FC9E-41B3-9AD4-1F3A1ADA833C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Insumos" sheetId="1" r:id="rId1"/>
@@ -360,7 +360,7 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -486,8 +486,8 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="A2:D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
validacion 4 repite trabajo en eso
</commit_message>
<xml_diff>
--- a/Data/Hoja de recursos.xlsx
+++ b/Data/Hoja de recursos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Desktop\importante\Generacion-Correo-Equipo-4\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E23437-A622-49FB-BC5C-1FCAAF872F19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC14A67-4E55-42AB-85C5-E8898E547459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6615" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2910" yWindow="2805" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Insumos" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
   <si>
     <t>Nombre</t>
   </si>
@@ -45,6 +45,9 @@
     <t>Hernández</t>
   </si>
   <si>
+    <t>Allisson</t>
+  </si>
+  <si>
     <t>Flores</t>
   </si>
   <si>
@@ -57,22 +60,16 @@
     <t>Correo Electrónico</t>
   </si>
   <si>
+    <t>Descripción</t>
+  </si>
+  <si>
     <t>ivan.garcia@beeckerco.com</t>
   </si>
   <si>
-    <t>ivan.hernandez@beeckerco.com</t>
-  </si>
-  <si>
-    <t>Descripción</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allisson </t>
-  </si>
-  <si>
-    <t>Nombre repetido</t>
-  </si>
-  <si>
-    <t>Sin apellido Paterno</t>
+    <t>allisson.flores@beeckerco.com</t>
+  </si>
+  <si>
+    <t>eunice.@beeckerco.com</t>
   </si>
 </sst>
 </file>
@@ -360,7 +357,7 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -404,18 +401,30 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="2" t="s">
@@ -432,9 +441,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="A2:C11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -444,17 +455,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -469,7 +495,9 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="A2:E9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -489,34 +517,20 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="A3" s="2"/>
       <c r="B3" s="3"/>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>